<commit_message>
removing outputs from Scripts folder
</commit_message>
<xml_diff>
--- a/RainfallRegionalisation/CheckingPercentileThresholds.xlsx
+++ b/RainfallRegionalisation/CheckingPercentileThresholds.xlsx
@@ -358,7 +358,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -388,8 +388,8 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f>20*90*24</f>
-        <v>43200</v>
+        <f>1*90*24</f>
+        <v>2160</v>
       </c>
       <c r="C2">
         <v>99</v>
@@ -404,7 +404,7 @@
       </c>
       <c r="F2">
         <f>E2*$A$2</f>
-        <v>432.0000000000004</v>
+        <v>21.600000000000019</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -421,7 +421,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F7" si="2">E3*$A$2</f>
-        <v>216.0000000000002</v>
+        <v>10.80000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -438,7 +438,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>129.60000000000011</v>
+        <v>6.4800000000000058</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -455,7 +455,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>43.199999999995242</v>
+        <v>2.1599999999997621</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -472,7 +472,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>21.599999999997621</v>
+        <v>1.0799999999998811</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -489,7 +489,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>4.3200000000043204</v>
+        <v>0.21600000000021602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
just changing variable names for running
</commit_message>
<xml_diff>
--- a/RainfallRegionalisation/CheckingPercentileThresholds.xlsx
+++ b/RainfallRegionalisation/CheckingPercentileThresholds.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Percentile</t>
   </si>
@@ -35,10 +35,19 @@
     <t>Remainder</t>
   </si>
   <si>
-    <t>No. of data points</t>
-  </si>
-  <si>
     <t>Total data points</t>
+  </si>
+  <si>
+    <t>Points in twenty years worth of JJAs</t>
+  </si>
+  <si>
+    <t>Points in one JJA</t>
+  </si>
+  <si>
+    <t>No. of data points in one JJA</t>
+  </si>
+  <si>
+    <t>No. of data points in twenty years of JJAs</t>
   </si>
 </sst>
 </file>
@@ -355,23 +364,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -383,113 +395,221 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>1*90*24</f>
         <v>2160</v>
       </c>
       <c r="C2">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D2">
-        <f>C2/100</f>
-        <v>0.99</v>
+        <f t="shared" ref="D2:D3" si="0">C2/100</f>
+        <v>0.95</v>
       </c>
       <c r="E2">
-        <f>1-D2</f>
-        <v>1.0000000000000009E-2</v>
+        <f t="shared" ref="E2:E3" si="1">1-D2</f>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="F2">
         <f>E2*$A$2</f>
+        <v>108.0000000000001</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G3" si="2">E2*$J$2</f>
+        <v>2160.0000000000018</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <f>20*90*24</f>
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>97</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3" si="3">E3*$A$2</f>
+        <v>64.800000000000054</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="2"/>
+        <v>1296.0000000000011</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <f>24*90</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <f>C4/100</f>
+        <v>0.99</v>
+      </c>
+      <c r="E4">
+        <f>1-D4</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="F4">
+        <f>E4*$A$2</f>
         <v>21.600000000000019</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C3">
+      <c r="G4">
+        <f>E4*$J$2</f>
+        <v>432.0000000000004</v>
+      </c>
+      <c r="J4">
+        <f>J2/J3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C5">
         <v>99.5</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D7" si="0">C3/100</f>
+      <c r="D5">
+        <f t="shared" ref="D5:D10" si="4">C5/100</f>
         <v>0.995</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="1">1-D3</f>
+      <c r="E5">
+        <f t="shared" ref="E5:E10" si="5">1-D5</f>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F7" si="2">E3*$A$2</f>
+      <c r="F5">
+        <f>E5*$A$2</f>
         <v>10.80000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C4">
-        <v>99.7</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.997</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000027E-3</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
-        <v>6.4800000000000058</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C5">
+      <c r="G5">
+        <f t="shared" ref="G5:G10" si="6">E5*$J$2</f>
+        <v>216.0000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>99.75</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="4"/>
+        <v>0.99750000000000005</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="5"/>
+        <v>2.4999999999999467E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F10" si="7">E6*$A$2</f>
+        <v>5.3999999999998849</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="6"/>
+        <v>107.9999999999977</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7">
         <v>99.9</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="D7">
+        <f t="shared" si="4"/>
         <v>0.99900000000000011</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
+      <c r="E7">
+        <f t="shared" si="5"/>
         <v>9.9999999999988987E-4</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
+      <c r="F7">
+        <f t="shared" si="7"/>
         <v>2.1599999999997621</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C6">
+      <c r="G7">
+        <f t="shared" si="6"/>
+        <v>43.199999999995242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C8">
         <v>99.95</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="D8">
+        <f t="shared" si="4"/>
         <v>0.99950000000000006</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
+      <c r="E8">
+        <f t="shared" si="5"/>
         <v>4.9999999999994493E-4</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
+      <c r="F8">
+        <f t="shared" si="7"/>
         <v>1.0799999999998811</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C7">
+      <c r="G8">
+        <f t="shared" si="6"/>
+        <v>21.599999999997621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C9">
         <v>99.99</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+      <c r="D9">
+        <f t="shared" si="4"/>
         <v>0.9998999999999999</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
+      <c r="E9">
+        <f t="shared" si="5"/>
         <v>1.0000000000010001E-4</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
+      <c r="F9">
+        <f t="shared" si="7"/>
         <v>0.21600000000021602</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="6"/>
+        <v>4.3200000000043204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="7"/>
+        <v>1080</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="6"/>
+        <v>21600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>